<commit_message>
Added DataView and report view script after integration
</commit_message>
<xml_diff>
--- a/Data/ReportView_SK_REG_COMPLETE_updated.xlsx
+++ b/Data/ReportView_SK_REG_COMPLETE_updated.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD06E7F-6C94-458B-98CB-28134C4FF153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5174A176-F5BA-4B58-9BAC-E19CC7799C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2958" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3213" uniqueCount="74">
   <si>
     <t>EMPID</t>
   </si>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I562"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A549" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="A165" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -5939,12 +5939,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="257" spans="1:5" s="3" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:6" s="3" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A257" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B257" s="4" t="s">
-        <v>63</v>
+      <c r="B257" t="s">
+        <v>6</v>
       </c>
       <c r="C257" s="3" t="s">
         <v>7</v>
@@ -5955,13 +5955,16 @@
       <c r="E257" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="258" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F257" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>67</v>
       </c>
-      <c r="B258" s="4" t="s">
-        <v>63</v>
+      <c r="B258" t="s">
+        <v>6</v>
       </c>
       <c r="C258" t="s">
         <v>11</v>
@@ -5972,13 +5975,16 @@
       <c r="E258" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="259" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F258" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>67</v>
       </c>
-      <c r="B259" s="4" t="s">
-        <v>63</v>
+      <c r="B259" t="s">
+        <v>6</v>
       </c>
       <c r="C259" t="s">
         <v>12</v>
@@ -5989,13 +5995,16 @@
       <c r="E259" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="260" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F259" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>67</v>
       </c>
-      <c r="B260" s="4" t="s">
-        <v>63</v>
+      <c r="B260" t="s">
+        <v>6</v>
       </c>
       <c r="C260" t="s">
         <v>13</v>
@@ -6006,13 +6015,16 @@
       <c r="E260" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="261" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F260" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>67</v>
       </c>
-      <c r="B261" s="4" t="s">
-        <v>63</v>
+      <c r="B261" t="s">
+        <v>6</v>
       </c>
       <c r="C261" t="s">
         <v>15</v>
@@ -6023,13 +6035,16 @@
       <c r="E261" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="262" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F261" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>67</v>
       </c>
-      <c r="B262" s="4" t="s">
-        <v>63</v>
+      <c r="B262" t="s">
+        <v>6</v>
       </c>
       <c r="C262" t="s">
         <v>16</v>
@@ -6040,13 +6055,16 @@
       <c r="E262" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="263" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F262" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>67</v>
       </c>
-      <c r="B263" s="4" t="s">
-        <v>63</v>
+      <c r="B263" t="s">
+        <v>6</v>
       </c>
       <c r="C263" t="s">
         <v>17</v>
@@ -6057,13 +6075,16 @@
       <c r="E263" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="264" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F263" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>67</v>
       </c>
-      <c r="B264" s="4" t="s">
-        <v>63</v>
+      <c r="B264" t="s">
+        <v>6</v>
       </c>
       <c r="C264" t="s">
         <v>18</v>
@@ -6074,13 +6095,16 @@
       <c r="E264" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="265" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F264" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>67</v>
       </c>
-      <c r="B265" s="4" t="s">
-        <v>63</v>
+      <c r="B265" t="s">
+        <v>6</v>
       </c>
       <c r="C265" t="s">
         <v>19</v>
@@ -6091,13 +6115,16 @@
       <c r="E265" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="266" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F265" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>67</v>
       </c>
-      <c r="B266" s="4" t="s">
-        <v>63</v>
+      <c r="B266" t="s">
+        <v>6</v>
       </c>
       <c r="C266" t="s">
         <v>20</v>
@@ -6108,13 +6135,16 @@
       <c r="E266" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="267" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F266" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>67</v>
       </c>
-      <c r="B267" s="4" t="s">
-        <v>63</v>
+      <c r="B267" t="s">
+        <v>6</v>
       </c>
       <c r="C267" t="s">
         <v>22</v>
@@ -6125,13 +6155,16 @@
       <c r="E267" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="268" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F267" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>67</v>
       </c>
-      <c r="B268" s="4" t="s">
-        <v>63</v>
+      <c r="B268" t="s">
+        <v>6</v>
       </c>
       <c r="C268" t="s">
         <v>23</v>
@@ -6142,13 +6175,16 @@
       <c r="E268" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="269" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F268" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>67</v>
       </c>
-      <c r="B269" s="4" t="s">
-        <v>63</v>
+      <c r="B269" t="s">
+        <v>6</v>
       </c>
       <c r="C269" t="s">
         <v>24</v>
@@ -6159,13 +6195,16 @@
       <c r="E269" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="270" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F269" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>67</v>
       </c>
-      <c r="B270" s="4" t="s">
-        <v>63</v>
+      <c r="B270" t="s">
+        <v>6</v>
       </c>
       <c r="C270" t="s">
         <v>25</v>
@@ -6176,13 +6215,16 @@
       <c r="E270" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="271" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F270" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>67</v>
       </c>
-      <c r="B271" s="4" t="s">
-        <v>63</v>
+      <c r="B271" t="s">
+        <v>6</v>
       </c>
       <c r="C271" t="s">
         <v>26</v>
@@ -6193,13 +6235,16 @@
       <c r="E271" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="272" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F271" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>67</v>
       </c>
-      <c r="B272" s="4" t="s">
-        <v>63</v>
+      <c r="B272" t="s">
+        <v>6</v>
       </c>
       <c r="C272" t="s">
         <v>27</v>
@@ -6210,13 +6255,16 @@
       <c r="E272" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="273" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F272" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>67</v>
       </c>
-      <c r="B273" s="4" t="s">
-        <v>63</v>
+      <c r="B273" t="s">
+        <v>6</v>
       </c>
       <c r="C273" t="s">
         <v>28</v>
@@ -6227,13 +6275,16 @@
       <c r="E273" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="274" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F273" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>67</v>
       </c>
-      <c r="B274" s="4" t="s">
-        <v>63</v>
+      <c r="B274" t="s">
+        <v>6</v>
       </c>
       <c r="C274" t="s">
         <v>29</v>
@@ -6244,13 +6295,16 @@
       <c r="E274" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="275" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F274" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>67</v>
       </c>
-      <c r="B275" s="4" t="s">
-        <v>63</v>
+      <c r="B275" t="s">
+        <v>6</v>
       </c>
       <c r="C275" t="s">
         <v>30</v>
@@ -6261,13 +6315,16 @@
       <c r="E275" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="276" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F275" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>67</v>
       </c>
-      <c r="B276" s="4" t="s">
-        <v>63</v>
+      <c r="B276" t="s">
+        <v>6</v>
       </c>
       <c r="C276" t="s">
         <v>31</v>
@@ -6278,13 +6335,16 @@
       <c r="E276" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="277" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F276" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>67</v>
       </c>
-      <c r="B277" s="4" t="s">
-        <v>63</v>
+      <c r="B277" t="s">
+        <v>6</v>
       </c>
       <c r="C277" t="s">
         <v>32</v>
@@ -6295,13 +6355,16 @@
       <c r="E277" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="278" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F277" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>67</v>
       </c>
-      <c r="B278" s="4" t="s">
-        <v>63</v>
+      <c r="B278" t="s">
+        <v>6</v>
       </c>
       <c r="C278" t="s">
         <v>33</v>
@@ -6312,13 +6375,16 @@
       <c r="E278" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="279" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F278" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>67</v>
       </c>
-      <c r="B279" s="4" t="s">
-        <v>63</v>
+      <c r="B279" t="s">
+        <v>6</v>
       </c>
       <c r="C279" t="s">
         <v>34</v>
@@ -6329,13 +6395,16 @@
       <c r="E279" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="280" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F279" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>67</v>
       </c>
-      <c r="B280" s="4" t="s">
-        <v>63</v>
+      <c r="B280" t="s">
+        <v>6</v>
       </c>
       <c r="C280" t="s">
         <v>35</v>
@@ -6346,13 +6415,16 @@
       <c r="E280" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="281" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F280" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>67</v>
       </c>
-      <c r="B281" s="4" t="s">
-        <v>63</v>
+      <c r="B281" t="s">
+        <v>6</v>
       </c>
       <c r="C281" t="s">
         <v>36</v>
@@ -6363,13 +6435,16 @@
       <c r="E281" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="282" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F281" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>67</v>
       </c>
-      <c r="B282" s="4" t="s">
-        <v>63</v>
+      <c r="B282" t="s">
+        <v>6</v>
       </c>
       <c r="C282" t="s">
         <v>37</v>
@@ -6380,13 +6455,16 @@
       <c r="E282" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="283" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F282" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>67</v>
       </c>
-      <c r="B283" s="4" t="s">
-        <v>63</v>
+      <c r="B283" t="s">
+        <v>6</v>
       </c>
       <c r="C283" t="s">
         <v>38</v>
@@ -6397,13 +6475,16 @@
       <c r="E283" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="284" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F283" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>67</v>
       </c>
-      <c r="B284" s="4" t="s">
-        <v>63</v>
+      <c r="B284" t="s">
+        <v>6</v>
       </c>
       <c r="C284" t="s">
         <v>39</v>
@@ -6414,13 +6495,16 @@
       <c r="E284" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="285" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F284" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>67</v>
       </c>
-      <c r="B285" s="4" t="s">
-        <v>63</v>
+      <c r="B285" t="s">
+        <v>6</v>
       </c>
       <c r="C285" t="s">
         <v>40</v>
@@ -6431,13 +6515,16 @@
       <c r="E285" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="286" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F285" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>67</v>
       </c>
-      <c r="B286" s="4" t="s">
-        <v>63</v>
+      <c r="B286" t="s">
+        <v>6</v>
       </c>
       <c r="C286" t="s">
         <v>41</v>
@@ -6448,13 +6535,16 @@
       <c r="E286" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="287" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F286" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>67</v>
       </c>
-      <c r="B287" s="4" t="s">
-        <v>63</v>
+      <c r="B287" t="s">
+        <v>6</v>
       </c>
       <c r="C287" t="s">
         <v>42</v>
@@ -6465,13 +6555,16 @@
       <c r="E287" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="288" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F287" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>67</v>
       </c>
-      <c r="B288" s="4" t="s">
-        <v>63</v>
+      <c r="B288" t="s">
+        <v>6</v>
       </c>
       <c r="C288" t="s">
         <v>43</v>
@@ -6482,13 +6575,16 @@
       <c r="E288" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="289" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F288" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>67</v>
       </c>
-      <c r="B289" s="4" t="s">
-        <v>63</v>
+      <c r="B289" t="s">
+        <v>6</v>
       </c>
       <c r="C289" t="s">
         <v>44</v>
@@ -6499,13 +6595,16 @@
       <c r="E289" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="290" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F289" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>67</v>
       </c>
-      <c r="B290" s="4" t="s">
-        <v>63</v>
+      <c r="B290" t="s">
+        <v>6</v>
       </c>
       <c r="C290" t="s">
         <v>45</v>
@@ -6516,13 +6615,16 @@
       <c r="E290" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="291" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F290" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>67</v>
       </c>
-      <c r="B291" s="4" t="s">
-        <v>63</v>
+      <c r="B291" t="s">
+        <v>6</v>
       </c>
       <c r="C291" t="s">
         <v>46</v>
@@ -6533,13 +6635,16 @@
       <c r="E291" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="292" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F291" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>67</v>
       </c>
-      <c r="B292" s="4" t="s">
-        <v>63</v>
+      <c r="B292" t="s">
+        <v>6</v>
       </c>
       <c r="C292" t="s">
         <v>47</v>
@@ -6550,13 +6655,16 @@
       <c r="E292" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="293" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F292" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>67</v>
       </c>
-      <c r="B293" s="4" t="s">
-        <v>63</v>
+      <c r="B293" t="s">
+        <v>6</v>
       </c>
       <c r="C293" t="s">
         <v>48</v>
@@ -6567,13 +6675,16 @@
       <c r="E293" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="294" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F293" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>67</v>
       </c>
-      <c r="B294" s="4" t="s">
-        <v>63</v>
+      <c r="B294" t="s">
+        <v>6</v>
       </c>
       <c r="C294" t="s">
         <v>49</v>
@@ -6584,13 +6695,16 @@
       <c r="E294" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="295" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F294" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>67</v>
       </c>
-      <c r="B295" s="4" t="s">
-        <v>63</v>
+      <c r="B295" t="s">
+        <v>6</v>
       </c>
       <c r="C295" t="s">
         <v>50</v>
@@ -6601,13 +6715,16 @@
       <c r="E295" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="296" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F295" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>67</v>
       </c>
-      <c r="B296" s="4" t="s">
-        <v>63</v>
+      <c r="B296" t="s">
+        <v>6</v>
       </c>
       <c r="C296" t="s">
         <v>51</v>
@@ -6618,13 +6735,16 @@
       <c r="E296" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="297" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F296" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>67</v>
       </c>
-      <c r="B297" s="4" t="s">
-        <v>63</v>
+      <c r="B297" t="s">
+        <v>6</v>
       </c>
       <c r="C297" t="s">
         <v>52</v>
@@ -6635,13 +6755,16 @@
       <c r="E297" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="298" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F297" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>67</v>
       </c>
-      <c r="B298" s="4" t="s">
-        <v>63</v>
+      <c r="B298" t="s">
+        <v>6</v>
       </c>
       <c r="C298" t="s">
         <v>53</v>
@@ -6652,13 +6775,16 @@
       <c r="E298" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="299" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F298" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>67</v>
       </c>
-      <c r="B299" s="4" t="s">
-        <v>63</v>
+      <c r="B299" t="s">
+        <v>6</v>
       </c>
       <c r="C299" t="s">
         <v>54</v>
@@ -6669,13 +6795,16 @@
       <c r="E299" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="300" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F299" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>67</v>
       </c>
-      <c r="B300" s="4" t="s">
-        <v>63</v>
+      <c r="B300" t="s">
+        <v>6</v>
       </c>
       <c r="C300" t="s">
         <v>55</v>
@@ -6686,13 +6815,16 @@
       <c r="E300" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="301" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F300" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>67</v>
       </c>
-      <c r="B301" s="4" t="s">
-        <v>63</v>
+      <c r="B301" t="s">
+        <v>6</v>
       </c>
       <c r="C301" t="s">
         <v>56</v>
@@ -6703,13 +6835,16 @@
       <c r="E301" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="302" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F301" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>67</v>
       </c>
-      <c r="B302" s="4" t="s">
-        <v>63</v>
+      <c r="B302" t="s">
+        <v>6</v>
       </c>
       <c r="C302" t="s">
         <v>57</v>
@@ -6720,13 +6855,16 @@
       <c r="E302" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="303" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F302" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>67</v>
       </c>
-      <c r="B303" s="4" t="s">
-        <v>63</v>
+      <c r="B303" t="s">
+        <v>6</v>
       </c>
       <c r="C303" t="s">
         <v>58</v>
@@ -6737,13 +6875,16 @@
       <c r="E303" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="304" spans="1:5" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F303" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>67</v>
       </c>
-      <c r="B304" s="4" t="s">
-        <v>63</v>
+      <c r="B304" t="s">
+        <v>6</v>
       </c>
       <c r="C304" t="s">
         <v>59</v>
@@ -6753,14 +6894,17 @@
       </c>
       <c r="E304" t="s">
         <v>9</v>
+      </c>
+      <c r="F304" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="305" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>67</v>
       </c>
-      <c r="B305" s="4" t="s">
-        <v>63</v>
+      <c r="B305" t="s">
+        <v>6</v>
       </c>
       <c r="C305" t="s">
         <v>60</v>
@@ -6770,14 +6914,17 @@
       </c>
       <c r="E305" t="s">
         <v>9</v>
+      </c>
+      <c r="F305" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="306" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>67</v>
       </c>
-      <c r="B306" s="4" t="s">
-        <v>63</v>
+      <c r="B306" t="s">
+        <v>6</v>
       </c>
       <c r="C306" t="s">
         <v>61</v>
@@ -6787,14 +6934,17 @@
       </c>
       <c r="E306" t="s">
         <v>9</v>
+      </c>
+      <c r="F306" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="307" spans="1:6" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>67</v>
       </c>
-      <c r="B307" s="4" t="s">
-        <v>63</v>
+      <c r="B307" t="s">
+        <v>6</v>
       </c>
       <c r="C307" t="s">
         <v>62</v>
@@ -6804,6 +6954,9 @@
       </c>
       <c r="E307" t="s">
         <v>9</v>
+      </c>
+      <c r="F307" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="308" spans="1:6" s="3" customFormat="1" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
@@ -7836,6 +7989,9 @@
       <c r="D359" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E359" t="s">
+        <v>9</v>
+      </c>
       <c r="F359" s="3" t="s">
         <v>10</v>
       </c>
@@ -7853,6 +8009,9 @@
       <c r="D360" t="s">
         <v>8</v>
       </c>
+      <c r="E360" t="s">
+        <v>9</v>
+      </c>
       <c r="F360" t="s">
         <v>10</v>
       </c>
@@ -7870,6 +8029,9 @@
       <c r="D361" t="s">
         <v>8</v>
       </c>
+      <c r="E361" t="s">
+        <v>9</v>
+      </c>
       <c r="F361" t="s">
         <v>10</v>
       </c>
@@ -7887,6 +8049,9 @@
       <c r="D362" t="s">
         <v>14</v>
       </c>
+      <c r="E362" t="s">
+        <v>9</v>
+      </c>
       <c r="F362" t="s">
         <v>10</v>
       </c>
@@ -7904,6 +8069,9 @@
       <c r="D363" t="s">
         <v>8</v>
       </c>
+      <c r="E363" t="s">
+        <v>9</v>
+      </c>
       <c r="F363" t="s">
         <v>10</v>
       </c>
@@ -7921,6 +8089,9 @@
       <c r="D364" t="s">
         <v>8</v>
       </c>
+      <c r="E364" t="s">
+        <v>9</v>
+      </c>
       <c r="F364" t="s">
         <v>10</v>
       </c>
@@ -7938,6 +8109,9 @@
       <c r="D365" t="s">
         <v>8</v>
       </c>
+      <c r="E365" t="s">
+        <v>9</v>
+      </c>
       <c r="F365" t="s">
         <v>10</v>
       </c>
@@ -7955,6 +8129,9 @@
       <c r="D366" t="s">
         <v>14</v>
       </c>
+      <c r="E366" t="s">
+        <v>9</v>
+      </c>
       <c r="F366" t="s">
         <v>10</v>
       </c>
@@ -7972,6 +8149,9 @@
       <c r="D367" t="s">
         <v>14</v>
       </c>
+      <c r="E367" t="s">
+        <v>9</v>
+      </c>
       <c r="F367" t="s">
         <v>10</v>
       </c>
@@ -7989,6 +8169,9 @@
       <c r="D368" t="s">
         <v>14</v>
       </c>
+      <c r="E368" t="s">
+        <v>9</v>
+      </c>
       <c r="F368" t="s">
         <v>21</v>
       </c>
@@ -8006,6 +8189,9 @@
       <c r="D369" t="s">
         <v>14</v>
       </c>
+      <c r="E369" t="s">
+        <v>9</v>
+      </c>
       <c r="F369" t="s">
         <v>21</v>
       </c>
@@ -8023,6 +8209,9 @@
       <c r="D370" t="s">
         <v>14</v>
       </c>
+      <c r="E370" t="s">
+        <v>9</v>
+      </c>
       <c r="F370" t="s">
         <v>10</v>
       </c>
@@ -8040,6 +8229,9 @@
       <c r="D371" t="s">
         <v>14</v>
       </c>
+      <c r="E371" t="s">
+        <v>9</v>
+      </c>
       <c r="F371" t="s">
         <v>10</v>
       </c>
@@ -8057,6 +8249,9 @@
       <c r="D372" t="s">
         <v>8</v>
       </c>
+      <c r="E372" t="s">
+        <v>9</v>
+      </c>
       <c r="F372" t="s">
         <v>10</v>
       </c>
@@ -8074,6 +8269,9 @@
       <c r="D373" t="s">
         <v>8</v>
       </c>
+      <c r="E373" t="s">
+        <v>9</v>
+      </c>
       <c r="F373" t="s">
         <v>10</v>
       </c>
@@ -8091,6 +8289,9 @@
       <c r="D374" t="s">
         <v>8</v>
       </c>
+      <c r="E374" t="s">
+        <v>9</v>
+      </c>
       <c r="F374" t="s">
         <v>10</v>
       </c>
@@ -8108,6 +8309,9 @@
       <c r="D375" t="s">
         <v>8</v>
       </c>
+      <c r="E375" t="s">
+        <v>9</v>
+      </c>
       <c r="F375" t="s">
         <v>10</v>
       </c>
@@ -8125,6 +8329,9 @@
       <c r="D376" t="s">
         <v>8</v>
       </c>
+      <c r="E376" t="s">
+        <v>9</v>
+      </c>
       <c r="F376" t="s">
         <v>10</v>
       </c>
@@ -8142,6 +8349,9 @@
       <c r="D377" t="s">
         <v>8</v>
       </c>
+      <c r="E377" t="s">
+        <v>9</v>
+      </c>
       <c r="F377" t="s">
         <v>10</v>
       </c>
@@ -8159,6 +8369,9 @@
       <c r="D378" t="s">
         <v>8</v>
       </c>
+      <c r="E378" t="s">
+        <v>9</v>
+      </c>
       <c r="F378" t="s">
         <v>10</v>
       </c>
@@ -8176,6 +8389,9 @@
       <c r="D379" t="s">
         <v>8</v>
       </c>
+      <c r="E379" t="s">
+        <v>9</v>
+      </c>
       <c r="F379" t="s">
         <v>10</v>
       </c>
@@ -8193,6 +8409,9 @@
       <c r="D380" t="s">
         <v>8</v>
       </c>
+      <c r="E380" t="s">
+        <v>9</v>
+      </c>
       <c r="F380" t="s">
         <v>10</v>
       </c>
@@ -8210,6 +8429,9 @@
       <c r="D381" t="s">
         <v>8</v>
       </c>
+      <c r="E381" t="s">
+        <v>9</v>
+      </c>
       <c r="F381" t="s">
         <v>10</v>
       </c>
@@ -8227,6 +8449,9 @@
       <c r="D382" t="s">
         <v>8</v>
       </c>
+      <c r="E382" t="s">
+        <v>9</v>
+      </c>
       <c r="F382" t="s">
         <v>10</v>
       </c>
@@ -8244,6 +8469,9 @@
       <c r="D383" t="s">
         <v>8</v>
       </c>
+      <c r="E383" t="s">
+        <v>9</v>
+      </c>
       <c r="F383" t="s">
         <v>10</v>
       </c>
@@ -8261,6 +8489,9 @@
       <c r="D384" t="s">
         <v>8</v>
       </c>
+      <c r="E384" t="s">
+        <v>9</v>
+      </c>
       <c r="F384" t="s">
         <v>10</v>
       </c>
@@ -8278,6 +8509,9 @@
       <c r="D385" t="s">
         <v>8</v>
       </c>
+      <c r="E385" t="s">
+        <v>9</v>
+      </c>
       <c r="F385" t="s">
         <v>10</v>
       </c>
@@ -8295,6 +8529,9 @@
       <c r="D386" t="s">
         <v>8</v>
       </c>
+      <c r="E386" t="s">
+        <v>9</v>
+      </c>
       <c r="F386" t="s">
         <v>10</v>
       </c>
@@ -8312,6 +8549,9 @@
       <c r="D387" t="s">
         <v>8</v>
       </c>
+      <c r="E387" t="s">
+        <v>9</v>
+      </c>
       <c r="F387" t="s">
         <v>10</v>
       </c>
@@ -8329,6 +8569,9 @@
       <c r="D388" t="s">
         <v>8</v>
       </c>
+      <c r="E388" t="s">
+        <v>9</v>
+      </c>
       <c r="F388" t="s">
         <v>10</v>
       </c>
@@ -8346,6 +8589,9 @@
       <c r="D389" t="s">
         <v>8</v>
       </c>
+      <c r="E389" t="s">
+        <v>9</v>
+      </c>
       <c r="F389" t="s">
         <v>10</v>
       </c>
@@ -8363,6 +8609,9 @@
       <c r="D390" t="s">
         <v>8</v>
       </c>
+      <c r="E390" t="s">
+        <v>9</v>
+      </c>
       <c r="F390" t="s">
         <v>10</v>
       </c>
@@ -8380,6 +8629,9 @@
       <c r="D391" t="s">
         <v>8</v>
       </c>
+      <c r="E391" t="s">
+        <v>9</v>
+      </c>
       <c r="F391" t="s">
         <v>10</v>
       </c>
@@ -8397,6 +8649,9 @@
       <c r="D392" t="s">
         <v>8</v>
       </c>
+      <c r="E392" t="s">
+        <v>9</v>
+      </c>
       <c r="F392" t="s">
         <v>10</v>
       </c>
@@ -8414,6 +8669,9 @@
       <c r="D393" t="s">
         <v>8</v>
       </c>
+      <c r="E393" t="s">
+        <v>9</v>
+      </c>
       <c r="F393" t="s">
         <v>10</v>
       </c>
@@ -8431,6 +8689,9 @@
       <c r="D394" t="s">
         <v>8</v>
       </c>
+      <c r="E394" t="s">
+        <v>9</v>
+      </c>
       <c r="F394" t="s">
         <v>10</v>
       </c>
@@ -8448,6 +8709,9 @@
       <c r="D395" t="s">
         <v>8</v>
       </c>
+      <c r="E395" t="s">
+        <v>9</v>
+      </c>
       <c r="F395" t="s">
         <v>10</v>
       </c>
@@ -8465,6 +8729,9 @@
       <c r="D396" t="s">
         <v>8</v>
       </c>
+      <c r="E396" t="s">
+        <v>9</v>
+      </c>
       <c r="F396" t="s">
         <v>10</v>
       </c>
@@ -8482,6 +8749,9 @@
       <c r="D397" t="s">
         <v>8</v>
       </c>
+      <c r="E397" t="s">
+        <v>9</v>
+      </c>
       <c r="F397" t="s">
         <v>10</v>
       </c>
@@ -8499,6 +8769,9 @@
       <c r="D398" t="s">
         <v>8</v>
       </c>
+      <c r="E398" t="s">
+        <v>9</v>
+      </c>
       <c r="F398" t="s">
         <v>10</v>
       </c>
@@ -8516,6 +8789,9 @@
       <c r="D399" t="s">
         <v>8</v>
       </c>
+      <c r="E399" t="s">
+        <v>9</v>
+      </c>
       <c r="F399" t="s">
         <v>10</v>
       </c>
@@ -8533,6 +8809,9 @@
       <c r="D400" t="s">
         <v>8</v>
       </c>
+      <c r="E400" t="s">
+        <v>9</v>
+      </c>
       <c r="F400" t="s">
         <v>10</v>
       </c>
@@ -8550,6 +8829,9 @@
       <c r="D401" t="s">
         <v>8</v>
       </c>
+      <c r="E401" t="s">
+        <v>9</v>
+      </c>
       <c r="F401" t="s">
         <v>10</v>
       </c>
@@ -8567,6 +8849,9 @@
       <c r="D402" t="s">
         <v>8</v>
       </c>
+      <c r="E402" t="s">
+        <v>9</v>
+      </c>
       <c r="F402" t="s">
         <v>10</v>
       </c>
@@ -8584,6 +8869,9 @@
       <c r="D403" t="s">
         <v>8</v>
       </c>
+      <c r="E403" t="s">
+        <v>9</v>
+      </c>
       <c r="F403" t="s">
         <v>10</v>
       </c>
@@ -8601,6 +8889,9 @@
       <c r="D404" t="s">
         <v>8</v>
       </c>
+      <c r="E404" t="s">
+        <v>9</v>
+      </c>
       <c r="F404" t="s">
         <v>10</v>
       </c>
@@ -8618,6 +8909,9 @@
       <c r="D405" t="s">
         <v>8</v>
       </c>
+      <c r="E405" t="s">
+        <v>9</v>
+      </c>
       <c r="F405" t="s">
         <v>10</v>
       </c>
@@ -8635,6 +8929,9 @@
       <c r="D406" t="s">
         <v>8</v>
       </c>
+      <c r="E406" t="s">
+        <v>9</v>
+      </c>
       <c r="F406" t="s">
         <v>10</v>
       </c>
@@ -8649,6 +8946,9 @@
       <c r="C407" t="s">
         <v>60</v>
       </c>
+      <c r="E407" t="s">
+        <v>9</v>
+      </c>
       <c r="F407" t="s">
         <v>21</v>
       </c>
@@ -8666,6 +8966,9 @@
       <c r="D408" t="s">
         <v>8</v>
       </c>
+      <c r="E408" t="s">
+        <v>9</v>
+      </c>
       <c r="F408" t="s">
         <v>10</v>
       </c>
@@ -8683,6 +8986,9 @@
       <c r="D409" t="s">
         <v>8</v>
       </c>
+      <c r="E409" t="s">
+        <v>9</v>
+      </c>
       <c r="F409" t="s">
         <v>10</v>
       </c>
@@ -8700,6 +9006,9 @@
       <c r="D410" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E410" t="s">
+        <v>9</v>
+      </c>
       <c r="F410" s="3" t="s">
         <v>10</v>
       </c>
@@ -8717,6 +9026,9 @@
       <c r="D411" t="s">
         <v>8</v>
       </c>
+      <c r="E411" t="s">
+        <v>9</v>
+      </c>
       <c r="F411" t="s">
         <v>10</v>
       </c>
@@ -8734,6 +9046,9 @@
       <c r="D412" t="s">
         <v>8</v>
       </c>
+      <c r="E412" t="s">
+        <v>9</v>
+      </c>
       <c r="F412" t="s">
         <v>10</v>
       </c>
@@ -8751,6 +9066,9 @@
       <c r="D413" t="s">
         <v>14</v>
       </c>
+      <c r="E413" t="s">
+        <v>9</v>
+      </c>
       <c r="F413" t="s">
         <v>10</v>
       </c>
@@ -8768,6 +9086,9 @@
       <c r="D414" t="s">
         <v>14</v>
       </c>
+      <c r="E414" t="s">
+        <v>9</v>
+      </c>
       <c r="F414" t="s">
         <v>10</v>
       </c>
@@ -8785,6 +9106,9 @@
       <c r="D415" t="s">
         <v>14</v>
       </c>
+      <c r="E415" t="s">
+        <v>9</v>
+      </c>
       <c r="F415" t="s">
         <v>10</v>
       </c>
@@ -8802,6 +9126,9 @@
       <c r="D416" t="s">
         <v>14</v>
       </c>
+      <c r="E416" t="s">
+        <v>9</v>
+      </c>
       <c r="F416" t="s">
         <v>10</v>
       </c>
@@ -8819,6 +9146,9 @@
       <c r="D417" t="s">
         <v>8</v>
       </c>
+      <c r="E417" t="s">
+        <v>9</v>
+      </c>
       <c r="F417" t="s">
         <v>10</v>
       </c>
@@ -8836,6 +9166,9 @@
       <c r="D418" t="s">
         <v>8</v>
       </c>
+      <c r="E418" t="s">
+        <v>9</v>
+      </c>
       <c r="F418" t="s">
         <v>10</v>
       </c>
@@ -8854,6 +9187,9 @@
       <c r="D419" t="s">
         <v>8</v>
       </c>
+      <c r="E419" t="s">
+        <v>9</v>
+      </c>
       <c r="F419" t="s">
         <v>10</v>
       </c>
@@ -8871,6 +9207,9 @@
       <c r="D420" t="s">
         <v>8</v>
       </c>
+      <c r="E420" t="s">
+        <v>9</v>
+      </c>
       <c r="F420" t="s">
         <v>10</v>
       </c>
@@ -8888,6 +9227,9 @@
       <c r="D421" t="s">
         <v>8</v>
       </c>
+      <c r="E421" t="s">
+        <v>9</v>
+      </c>
       <c r="F421" t="s">
         <v>10</v>
       </c>
@@ -8905,6 +9247,9 @@
       <c r="D422" t="s">
         <v>8</v>
       </c>
+      <c r="E422" t="s">
+        <v>9</v>
+      </c>
       <c r="F422" t="s">
         <v>10</v>
       </c>
@@ -8922,6 +9267,9 @@
       <c r="D423" t="s">
         <v>8</v>
       </c>
+      <c r="E423" t="s">
+        <v>9</v>
+      </c>
       <c r="F423" t="s">
         <v>10</v>
       </c>
@@ -8939,6 +9287,9 @@
       <c r="D424" t="s">
         <v>8</v>
       </c>
+      <c r="E424" t="s">
+        <v>9</v>
+      </c>
       <c r="F424" t="s">
         <v>10</v>
       </c>
@@ -8956,6 +9307,9 @@
       <c r="D425" t="s">
         <v>8</v>
       </c>
+      <c r="E425" t="s">
+        <v>9</v>
+      </c>
       <c r="F425" t="s">
         <v>10</v>
       </c>
@@ -8973,6 +9327,9 @@
       <c r="D426" t="s">
         <v>8</v>
       </c>
+      <c r="E426" t="s">
+        <v>9</v>
+      </c>
       <c r="F426" t="s">
         <v>10</v>
       </c>
@@ -8990,6 +9347,9 @@
       <c r="D427" t="s">
         <v>8</v>
       </c>
+      <c r="E427" t="s">
+        <v>9</v>
+      </c>
       <c r="F427" t="s">
         <v>10</v>
       </c>
@@ -9007,6 +9367,9 @@
       <c r="D428" t="s">
         <v>8</v>
       </c>
+      <c r="E428" t="s">
+        <v>9</v>
+      </c>
       <c r="F428" t="s">
         <v>10</v>
       </c>
@@ -9024,6 +9387,9 @@
       <c r="D429" t="s">
         <v>8</v>
       </c>
+      <c r="E429" t="s">
+        <v>9</v>
+      </c>
       <c r="F429" t="s">
         <v>10</v>
       </c>
@@ -9041,6 +9407,9 @@
       <c r="D430" t="s">
         <v>8</v>
       </c>
+      <c r="E430" t="s">
+        <v>9</v>
+      </c>
       <c r="F430" t="s">
         <v>10</v>
       </c>
@@ -9058,6 +9427,9 @@
       <c r="D431" t="s">
         <v>8</v>
       </c>
+      <c r="E431" t="s">
+        <v>9</v>
+      </c>
       <c r="F431" t="s">
         <v>10</v>
       </c>
@@ -9075,6 +9447,9 @@
       <c r="D432" t="s">
         <v>8</v>
       </c>
+      <c r="E432" t="s">
+        <v>9</v>
+      </c>
       <c r="F432" t="s">
         <v>10</v>
       </c>
@@ -9092,6 +9467,9 @@
       <c r="D433" t="s">
         <v>8</v>
       </c>
+      <c r="E433" t="s">
+        <v>9</v>
+      </c>
       <c r="F433" t="s">
         <v>10</v>
       </c>
@@ -9109,6 +9487,9 @@
       <c r="D434" t="s">
         <v>8</v>
       </c>
+      <c r="E434" t="s">
+        <v>9</v>
+      </c>
       <c r="F434" t="s">
         <v>10</v>
       </c>
@@ -9126,6 +9507,9 @@
       <c r="D435" t="s">
         <v>8</v>
       </c>
+      <c r="E435" t="s">
+        <v>9</v>
+      </c>
       <c r="F435" t="s">
         <v>10</v>
       </c>
@@ -9143,6 +9527,9 @@
       <c r="D436" t="s">
         <v>8</v>
       </c>
+      <c r="E436" t="s">
+        <v>9</v>
+      </c>
       <c r="F436" t="s">
         <v>10</v>
       </c>
@@ -9160,6 +9547,9 @@
       <c r="D437" t="s">
         <v>8</v>
       </c>
+      <c r="E437" t="s">
+        <v>9</v>
+      </c>
       <c r="F437" t="s">
         <v>10</v>
       </c>
@@ -9177,6 +9567,9 @@
       <c r="D438" t="s">
         <v>8</v>
       </c>
+      <c r="E438" t="s">
+        <v>9</v>
+      </c>
       <c r="F438" t="s">
         <v>10</v>
       </c>
@@ -9194,6 +9587,9 @@
       <c r="D439" t="s">
         <v>8</v>
       </c>
+      <c r="E439" t="s">
+        <v>9</v>
+      </c>
       <c r="F439" t="s">
         <v>10</v>
       </c>
@@ -9211,6 +9607,9 @@
       <c r="D440" t="s">
         <v>8</v>
       </c>
+      <c r="E440" t="s">
+        <v>9</v>
+      </c>
       <c r="F440" t="s">
         <v>10</v>
       </c>
@@ -9228,6 +9627,9 @@
       <c r="D441" t="s">
         <v>8</v>
       </c>
+      <c r="E441" t="s">
+        <v>9</v>
+      </c>
       <c r="F441" t="s">
         <v>10</v>
       </c>
@@ -9245,6 +9647,9 @@
       <c r="D442" t="s">
         <v>8</v>
       </c>
+      <c r="E442" t="s">
+        <v>9</v>
+      </c>
       <c r="F442" t="s">
         <v>10</v>
       </c>
@@ -9262,6 +9667,9 @@
       <c r="D443" t="s">
         <v>8</v>
       </c>
+      <c r="E443" t="s">
+        <v>9</v>
+      </c>
       <c r="F443" t="s">
         <v>10</v>
       </c>
@@ -9279,6 +9687,9 @@
       <c r="D444" t="s">
         <v>8</v>
       </c>
+      <c r="E444" t="s">
+        <v>9</v>
+      </c>
       <c r="F444" t="s">
         <v>10</v>
       </c>
@@ -9296,6 +9707,9 @@
       <c r="D445" t="s">
         <v>8</v>
       </c>
+      <c r="E445" t="s">
+        <v>9</v>
+      </c>
       <c r="F445" t="s">
         <v>10</v>
       </c>
@@ -9313,6 +9727,9 @@
       <c r="D446" t="s">
         <v>8</v>
       </c>
+      <c r="E446" t="s">
+        <v>9</v>
+      </c>
       <c r="F446" t="s">
         <v>10</v>
       </c>
@@ -9330,6 +9747,9 @@
       <c r="D447" t="s">
         <v>8</v>
       </c>
+      <c r="E447" t="s">
+        <v>9</v>
+      </c>
       <c r="F447" t="s">
         <v>10</v>
       </c>
@@ -9347,6 +9767,9 @@
       <c r="D448" t="s">
         <v>8</v>
       </c>
+      <c r="E448" t="s">
+        <v>9</v>
+      </c>
       <c r="F448" t="s">
         <v>10</v>
       </c>
@@ -9364,6 +9787,9 @@
       <c r="D449" t="s">
         <v>8</v>
       </c>
+      <c r="E449" t="s">
+        <v>9</v>
+      </c>
       <c r="F449" t="s">
         <v>10</v>
       </c>
@@ -9381,6 +9807,9 @@
       <c r="D450" t="s">
         <v>8</v>
       </c>
+      <c r="E450" t="s">
+        <v>9</v>
+      </c>
       <c r="F450" t="s">
         <v>10</v>
       </c>
@@ -9398,6 +9827,9 @@
       <c r="D451" t="s">
         <v>8</v>
       </c>
+      <c r="E451" t="s">
+        <v>9</v>
+      </c>
       <c r="F451" t="s">
         <v>10</v>
       </c>
@@ -9415,6 +9847,9 @@
       <c r="D452" t="s">
         <v>8</v>
       </c>
+      <c r="E452" t="s">
+        <v>9</v>
+      </c>
       <c r="F452" t="s">
         <v>10</v>
       </c>
@@ -9432,6 +9867,9 @@
       <c r="D453" t="s">
         <v>8</v>
       </c>
+      <c r="E453" t="s">
+        <v>9</v>
+      </c>
       <c r="F453" t="s">
         <v>10</v>
       </c>
@@ -9449,6 +9887,9 @@
       <c r="D454" t="s">
         <v>8</v>
       </c>
+      <c r="E454" t="s">
+        <v>9</v>
+      </c>
       <c r="F454" t="s">
         <v>10</v>
       </c>
@@ -9466,6 +9907,9 @@
       <c r="D455" t="s">
         <v>8</v>
       </c>
+      <c r="E455" t="s">
+        <v>9</v>
+      </c>
       <c r="F455" t="s">
         <v>10</v>
       </c>
@@ -9483,6 +9927,9 @@
       <c r="D456" t="s">
         <v>8</v>
       </c>
+      <c r="E456" t="s">
+        <v>9</v>
+      </c>
       <c r="F456" t="s">
         <v>10</v>
       </c>
@@ -9500,6 +9947,9 @@
       <c r="D457" t="s">
         <v>8</v>
       </c>
+      <c r="E457" t="s">
+        <v>9</v>
+      </c>
       <c r="F457" t="s">
         <v>10</v>
       </c>
@@ -9514,6 +9964,9 @@
       <c r="C458" t="s">
         <v>60</v>
       </c>
+      <c r="E458" t="s">
+        <v>9</v>
+      </c>
       <c r="F458" t="s">
         <v>21</v>
       </c>
@@ -9531,6 +9984,9 @@
       <c r="D459" t="s">
         <v>8</v>
       </c>
+      <c r="E459" t="s">
+        <v>9</v>
+      </c>
       <c r="F459" t="s">
         <v>10</v>
       </c>
@@ -9548,6 +10004,9 @@
       <c r="D460" t="s">
         <v>8</v>
       </c>
+      <c r="E460" t="s">
+        <v>9</v>
+      </c>
       <c r="F460" t="s">
         <v>10</v>
       </c>
@@ -9565,6 +10024,9 @@
       <c r="D461" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="E461" t="s">
+        <v>9</v>
+      </c>
       <c r="F461" s="3" t="s">
         <v>10</v>
       </c>
@@ -9582,6 +10044,9 @@
       <c r="D462" t="s">
         <v>14</v>
       </c>
+      <c r="E462" t="s">
+        <v>9</v>
+      </c>
       <c r="F462" t="s">
         <v>10</v>
       </c>
@@ -9599,6 +10064,9 @@
       <c r="D463" t="s">
         <v>14</v>
       </c>
+      <c r="E463" t="s">
+        <v>9</v>
+      </c>
       <c r="F463" t="s">
         <v>21</v>
       </c>
@@ -9616,6 +10084,9 @@
       <c r="D464" t="s">
         <v>14</v>
       </c>
+      <c r="E464" t="s">
+        <v>9</v>
+      </c>
       <c r="F464" t="s">
         <v>10</v>
       </c>
@@ -9633,6 +10104,9 @@
       <c r="D465" t="s">
         <v>14</v>
       </c>
+      <c r="E465" t="s">
+        <v>9</v>
+      </c>
       <c r="F465" t="s">
         <v>10</v>
       </c>
@@ -9650,6 +10124,9 @@
       <c r="D466" t="s">
         <v>14</v>
       </c>
+      <c r="E466" t="s">
+        <v>9</v>
+      </c>
       <c r="F466" t="s">
         <v>10</v>
       </c>
@@ -9667,6 +10144,9 @@
       <c r="D467" t="s">
         <v>14</v>
       </c>
+      <c r="E467" t="s">
+        <v>9</v>
+      </c>
       <c r="F467" t="s">
         <v>10</v>
       </c>
@@ -9684,6 +10164,9 @@
       <c r="D468" t="s">
         <v>14</v>
       </c>
+      <c r="E468" t="s">
+        <v>9</v>
+      </c>
       <c r="F468" t="s">
         <v>10</v>
       </c>
@@ -9701,6 +10184,9 @@
       <c r="D469" t="s">
         <v>14</v>
       </c>
+      <c r="E469" t="s">
+        <v>9</v>
+      </c>
       <c r="F469" t="s">
         <v>10</v>
       </c>
@@ -9718,6 +10204,9 @@
       <c r="D470" t="s">
         <v>14</v>
       </c>
+      <c r="E470" t="s">
+        <v>9</v>
+      </c>
       <c r="F470" t="s">
         <v>21</v>
       </c>
@@ -9735,6 +10224,9 @@
       <c r="D471" t="s">
         <v>14</v>
       </c>
+      <c r="E471" t="s">
+        <v>9</v>
+      </c>
       <c r="F471" t="s">
         <v>21</v>
       </c>
@@ -9752,6 +10244,9 @@
       <c r="D472" t="s">
         <v>14</v>
       </c>
+      <c r="E472" t="s">
+        <v>9</v>
+      </c>
       <c r="F472" t="s">
         <v>10</v>
       </c>
@@ -9769,6 +10264,9 @@
       <c r="D473" t="s">
         <v>14</v>
       </c>
+      <c r="E473" t="s">
+        <v>9</v>
+      </c>
       <c r="F473" t="s">
         <v>10</v>
       </c>
@@ -9786,6 +10284,9 @@
       <c r="D474" t="s">
         <v>14</v>
       </c>
+      <c r="E474" t="s">
+        <v>9</v>
+      </c>
       <c r="F474" t="s">
         <v>21</v>
       </c>
@@ -9803,6 +10304,9 @@
       <c r="D475" t="s">
         <v>14</v>
       </c>
+      <c r="E475" t="s">
+        <v>9</v>
+      </c>
       <c r="F475" t="s">
         <v>21</v>
       </c>
@@ -9820,6 +10324,9 @@
       <c r="D476" t="s">
         <v>14</v>
       </c>
+      <c r="E476" t="s">
+        <v>9</v>
+      </c>
       <c r="F476" t="s">
         <v>10</v>
       </c>
@@ -9837,6 +10344,9 @@
       <c r="D477" t="s">
         <v>14</v>
       </c>
+      <c r="E477" t="s">
+        <v>9</v>
+      </c>
       <c r="F477" t="s">
         <v>10</v>
       </c>
@@ -9854,6 +10364,9 @@
       <c r="D478" t="s">
         <v>14</v>
       </c>
+      <c r="E478" t="s">
+        <v>9</v>
+      </c>
       <c r="F478" t="s">
         <v>10</v>
       </c>
@@ -9871,6 +10384,9 @@
       <c r="D479" t="s">
         <v>14</v>
       </c>
+      <c r="E479" t="s">
+        <v>9</v>
+      </c>
       <c r="F479" t="s">
         <v>10</v>
       </c>
@@ -9888,6 +10404,9 @@
       <c r="D480" t="s">
         <v>14</v>
       </c>
+      <c r="E480" t="s">
+        <v>9</v>
+      </c>
       <c r="F480" t="s">
         <v>21</v>
       </c>
@@ -9905,6 +10424,9 @@
       <c r="D481" t="s">
         <v>14</v>
       </c>
+      <c r="E481" t="s">
+        <v>9</v>
+      </c>
       <c r="F481" t="s">
         <v>10</v>
       </c>
@@ -9922,6 +10444,9 @@
       <c r="D482" t="s">
         <v>14</v>
       </c>
+      <c r="E482" t="s">
+        <v>9</v>
+      </c>
       <c r="F482" t="s">
         <v>10</v>
       </c>
@@ -9939,6 +10464,9 @@
       <c r="D483" t="s">
         <v>14</v>
       </c>
+      <c r="E483" t="s">
+        <v>9</v>
+      </c>
       <c r="F483" t="s">
         <v>10</v>
       </c>
@@ -9956,6 +10484,9 @@
       <c r="D484" t="s">
         <v>14</v>
       </c>
+      <c r="E484" t="s">
+        <v>9</v>
+      </c>
       <c r="F484" t="s">
         <v>21</v>
       </c>
@@ -9973,6 +10504,9 @@
       <c r="D485" t="s">
         <v>14</v>
       </c>
+      <c r="E485" t="s">
+        <v>9</v>
+      </c>
       <c r="F485" t="s">
         <v>10</v>
       </c>
@@ -9990,6 +10524,9 @@
       <c r="D486" t="s">
         <v>14</v>
       </c>
+      <c r="E486" t="s">
+        <v>9</v>
+      </c>
       <c r="F486" t="s">
         <v>10</v>
       </c>
@@ -10007,6 +10544,9 @@
       <c r="D487" t="s">
         <v>14</v>
       </c>
+      <c r="E487" t="s">
+        <v>9</v>
+      </c>
       <c r="F487" t="s">
         <v>10</v>
       </c>
@@ -10024,6 +10564,9 @@
       <c r="D488" t="s">
         <v>14</v>
       </c>
+      <c r="E488" t="s">
+        <v>9</v>
+      </c>
       <c r="F488" t="s">
         <v>10</v>
       </c>
@@ -10041,6 +10584,9 @@
       <c r="D489" t="s">
         <v>14</v>
       </c>
+      <c r="E489" t="s">
+        <v>9</v>
+      </c>
       <c r="F489" t="s">
         <v>10</v>
       </c>
@@ -10058,6 +10604,9 @@
       <c r="D490" t="s">
         <v>14</v>
       </c>
+      <c r="E490" t="s">
+        <v>9</v>
+      </c>
       <c r="F490" t="s">
         <v>10</v>
       </c>
@@ -10075,6 +10624,9 @@
       <c r="D491" t="s">
         <v>14</v>
       </c>
+      <c r="E491" t="s">
+        <v>9</v>
+      </c>
       <c r="F491" t="s">
         <v>10</v>
       </c>
@@ -10092,6 +10644,9 @@
       <c r="D492" t="s">
         <v>14</v>
       </c>
+      <c r="E492" t="s">
+        <v>9</v>
+      </c>
       <c r="F492" t="s">
         <v>10</v>
       </c>
@@ -10109,6 +10664,9 @@
       <c r="D493" t="s">
         <v>14</v>
       </c>
+      <c r="E493" t="s">
+        <v>9</v>
+      </c>
       <c r="F493" t="s">
         <v>10</v>
       </c>
@@ -10126,6 +10684,9 @@
       <c r="D494" t="s">
         <v>14</v>
       </c>
+      <c r="E494" t="s">
+        <v>9</v>
+      </c>
       <c r="F494" t="s">
         <v>10</v>
       </c>
@@ -10143,6 +10704,9 @@
       <c r="D495" t="s">
         <v>14</v>
       </c>
+      <c r="E495" t="s">
+        <v>9</v>
+      </c>
       <c r="F495" t="s">
         <v>21</v>
       </c>
@@ -10160,6 +10724,9 @@
       <c r="D496" t="s">
         <v>14</v>
       </c>
+      <c r="E496" t="s">
+        <v>9</v>
+      </c>
       <c r="F496" t="s">
         <v>10</v>
       </c>
@@ -10177,6 +10744,9 @@
       <c r="D497" t="s">
         <v>14</v>
       </c>
+      <c r="E497" t="s">
+        <v>9</v>
+      </c>
       <c r="F497" t="s">
         <v>10</v>
       </c>
@@ -10194,6 +10764,9 @@
       <c r="D498" t="s">
         <v>14</v>
       </c>
+      <c r="E498" t="s">
+        <v>9</v>
+      </c>
       <c r="F498" t="s">
         <v>10</v>
       </c>
@@ -10211,6 +10784,9 @@
       <c r="D499" t="s">
         <v>14</v>
       </c>
+      <c r="E499" t="s">
+        <v>9</v>
+      </c>
       <c r="F499" t="s">
         <v>10</v>
       </c>
@@ -10228,6 +10804,9 @@
       <c r="D500" t="s">
         <v>14</v>
       </c>
+      <c r="E500" t="s">
+        <v>9</v>
+      </c>
       <c r="F500" t="s">
         <v>21</v>
       </c>
@@ -10245,6 +10824,9 @@
       <c r="D501" t="s">
         <v>14</v>
       </c>
+      <c r="E501" t="s">
+        <v>9</v>
+      </c>
       <c r="F501" t="s">
         <v>10</v>
       </c>
@@ -10262,6 +10844,9 @@
       <c r="D502" t="s">
         <v>14</v>
       </c>
+      <c r="E502" t="s">
+        <v>9</v>
+      </c>
       <c r="F502" t="s">
         <v>10</v>
       </c>
@@ -10279,6 +10864,9 @@
       <c r="D503" t="s">
         <v>14</v>
       </c>
+      <c r="E503" t="s">
+        <v>9</v>
+      </c>
       <c r="F503" t="s">
         <v>10</v>
       </c>
@@ -10296,6 +10884,9 @@
       <c r="D504" t="s">
         <v>14</v>
       </c>
+      <c r="E504" t="s">
+        <v>9</v>
+      </c>
       <c r="F504" t="s">
         <v>10</v>
       </c>
@@ -10313,6 +10904,9 @@
       <c r="D505" t="s">
         <v>14</v>
       </c>
+      <c r="E505" t="s">
+        <v>9</v>
+      </c>
       <c r="F505" t="s">
         <v>10</v>
       </c>
@@ -10330,6 +10924,9 @@
       <c r="D506" t="s">
         <v>14</v>
       </c>
+      <c r="E506" t="s">
+        <v>9</v>
+      </c>
       <c r="F506" t="s">
         <v>10</v>
       </c>
@@ -10347,6 +10944,9 @@
       <c r="D507" t="s">
         <v>14</v>
       </c>
+      <c r="E507" t="s">
+        <v>9</v>
+      </c>
       <c r="F507" t="s">
         <v>10</v>
       </c>
@@ -10364,6 +10964,9 @@
       <c r="D508" t="s">
         <v>14</v>
       </c>
+      <c r="E508" t="s">
+        <v>9</v>
+      </c>
       <c r="F508" t="s">
         <v>10</v>
       </c>
@@ -10381,6 +10984,9 @@
       <c r="D509" t="s">
         <v>14</v>
       </c>
+      <c r="E509" t="s">
+        <v>9</v>
+      </c>
       <c r="F509" t="s">
         <v>10</v>
       </c>
@@ -10398,6 +11004,9 @@
       <c r="D510" t="s">
         <v>14</v>
       </c>
+      <c r="E510" t="s">
+        <v>9</v>
+      </c>
       <c r="F510" t="s">
         <v>10</v>
       </c>
@@ -10415,6 +11024,9 @@
       <c r="D511" t="s">
         <v>14</v>
       </c>
+      <c r="E511" t="s">
+        <v>9</v>
+      </c>
       <c r="F511" t="s">
         <v>10</v>
       </c>
@@ -10432,6 +11044,9 @@
       <c r="D512" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="E512" t="s">
+        <v>9</v>
+      </c>
       <c r="F512" s="3" t="s">
         <v>10</v>
       </c>
@@ -10449,6 +11064,9 @@
       <c r="D513" t="s">
         <v>14</v>
       </c>
+      <c r="E513" t="s">
+        <v>9</v>
+      </c>
       <c r="F513" t="s">
         <v>10</v>
       </c>
@@ -10466,6 +11084,9 @@
       <c r="D514" t="s">
         <v>14</v>
       </c>
+      <c r="E514" t="s">
+        <v>9</v>
+      </c>
       <c r="F514" t="s">
         <v>21</v>
       </c>
@@ -10483,6 +11104,9 @@
       <c r="D515" t="s">
         <v>14</v>
       </c>
+      <c r="E515" t="s">
+        <v>9</v>
+      </c>
       <c r="F515" t="s">
         <v>10</v>
       </c>
@@ -10500,6 +11124,9 @@
       <c r="D516" t="s">
         <v>14</v>
       </c>
+      <c r="E516" t="s">
+        <v>9</v>
+      </c>
       <c r="F516" t="s">
         <v>10</v>
       </c>
@@ -10517,6 +11144,9 @@
       <c r="D517" t="s">
         <v>14</v>
       </c>
+      <c r="E517" t="s">
+        <v>9</v>
+      </c>
       <c r="F517" t="s">
         <v>10</v>
       </c>
@@ -10534,6 +11164,9 @@
       <c r="D518" t="s">
         <v>14</v>
       </c>
+      <c r="E518" t="s">
+        <v>9</v>
+      </c>
       <c r="F518" t="s">
         <v>10</v>
       </c>
@@ -10551,6 +11184,9 @@
       <c r="D519" t="s">
         <v>14</v>
       </c>
+      <c r="E519" t="s">
+        <v>9</v>
+      </c>
       <c r="F519" t="s">
         <v>10</v>
       </c>
@@ -10568,6 +11204,9 @@
       <c r="D520" t="s">
         <v>14</v>
       </c>
+      <c r="E520" t="s">
+        <v>9</v>
+      </c>
       <c r="F520" t="s">
         <v>10</v>
       </c>
@@ -10585,6 +11224,9 @@
       <c r="D521" t="s">
         <v>14</v>
       </c>
+      <c r="E521" t="s">
+        <v>9</v>
+      </c>
       <c r="F521" t="s">
         <v>21</v>
       </c>
@@ -10602,6 +11244,9 @@
       <c r="D522" t="s">
         <v>14</v>
       </c>
+      <c r="E522" t="s">
+        <v>9</v>
+      </c>
       <c r="F522" t="s">
         <v>21</v>
       </c>
@@ -10619,6 +11264,9 @@
       <c r="D523" t="s">
         <v>14</v>
       </c>
+      <c r="E523" t="s">
+        <v>9</v>
+      </c>
       <c r="F523" t="s">
         <v>10</v>
       </c>
@@ -10636,6 +11284,9 @@
       <c r="D524" t="s">
         <v>14</v>
       </c>
+      <c r="E524" t="s">
+        <v>9</v>
+      </c>
       <c r="F524" t="s">
         <v>10</v>
       </c>
@@ -10653,6 +11304,9 @@
       <c r="D525" t="s">
         <v>14</v>
       </c>
+      <c r="E525" t="s">
+        <v>9</v>
+      </c>
       <c r="F525" t="s">
         <v>21</v>
       </c>
@@ -10670,6 +11324,9 @@
       <c r="D526" t="s">
         <v>14</v>
       </c>
+      <c r="E526" t="s">
+        <v>9</v>
+      </c>
       <c r="F526" t="s">
         <v>21</v>
       </c>
@@ -10687,6 +11344,9 @@
       <c r="D527" t="s">
         <v>14</v>
       </c>
+      <c r="E527" t="s">
+        <v>9</v>
+      </c>
       <c r="F527" t="s">
         <v>10</v>
       </c>
@@ -10704,6 +11364,9 @@
       <c r="D528" t="s">
         <v>14</v>
       </c>
+      <c r="E528" t="s">
+        <v>9</v>
+      </c>
       <c r="F528" t="s">
         <v>10</v>
       </c>
@@ -10721,6 +11384,9 @@
       <c r="D529" t="s">
         <v>14</v>
       </c>
+      <c r="E529" t="s">
+        <v>9</v>
+      </c>
       <c r="F529" t="s">
         <v>10</v>
       </c>
@@ -10738,6 +11404,9 @@
       <c r="D530" t="s">
         <v>14</v>
       </c>
+      <c r="E530" t="s">
+        <v>9</v>
+      </c>
       <c r="F530" t="s">
         <v>10</v>
       </c>
@@ -10755,6 +11424,9 @@
       <c r="D531" t="s">
         <v>14</v>
       </c>
+      <c r="E531" t="s">
+        <v>9</v>
+      </c>
       <c r="F531" t="s">
         <v>21</v>
       </c>
@@ -10772,6 +11444,9 @@
       <c r="D532" t="s">
         <v>14</v>
       </c>
+      <c r="E532" t="s">
+        <v>9</v>
+      </c>
       <c r="F532" t="s">
         <v>10</v>
       </c>
@@ -10789,6 +11464,9 @@
       <c r="D533" t="s">
         <v>14</v>
       </c>
+      <c r="E533" t="s">
+        <v>9</v>
+      </c>
       <c r="F533" t="s">
         <v>10</v>
       </c>
@@ -10806,6 +11484,9 @@
       <c r="D534" t="s">
         <v>14</v>
       </c>
+      <c r="E534" t="s">
+        <v>9</v>
+      </c>
       <c r="F534" t="s">
         <v>10</v>
       </c>
@@ -10823,6 +11504,9 @@
       <c r="D535" t="s">
         <v>14</v>
       </c>
+      <c r="E535" t="s">
+        <v>9</v>
+      </c>
       <c r="F535" t="s">
         <v>21</v>
       </c>
@@ -10840,6 +11524,9 @@
       <c r="D536" t="s">
         <v>14</v>
       </c>
+      <c r="E536" t="s">
+        <v>9</v>
+      </c>
       <c r="F536" t="s">
         <v>10</v>
       </c>
@@ -10857,6 +11544,9 @@
       <c r="D537" t="s">
         <v>14</v>
       </c>
+      <c r="E537" t="s">
+        <v>9</v>
+      </c>
       <c r="F537" t="s">
         <v>10</v>
       </c>
@@ -10874,6 +11564,9 @@
       <c r="D538" t="s">
         <v>14</v>
       </c>
+      <c r="E538" t="s">
+        <v>9</v>
+      </c>
       <c r="F538" t="s">
         <v>10</v>
       </c>
@@ -10891,6 +11584,9 @@
       <c r="D539" t="s">
         <v>14</v>
       </c>
+      <c r="E539" t="s">
+        <v>9</v>
+      </c>
       <c r="F539" t="s">
         <v>10</v>
       </c>
@@ -10908,6 +11604,9 @@
       <c r="D540" t="s">
         <v>14</v>
       </c>
+      <c r="E540" t="s">
+        <v>9</v>
+      </c>
       <c r="F540" t="s">
         <v>10</v>
       </c>
@@ -10925,6 +11624,9 @@
       <c r="D541" t="s">
         <v>14</v>
       </c>
+      <c r="E541" t="s">
+        <v>9</v>
+      </c>
       <c r="F541" t="s">
         <v>10</v>
       </c>
@@ -10942,6 +11644,9 @@
       <c r="D542" t="s">
         <v>14</v>
       </c>
+      <c r="E542" t="s">
+        <v>9</v>
+      </c>
       <c r="F542" t="s">
         <v>10</v>
       </c>
@@ -10959,6 +11664,9 @@
       <c r="D543" t="s">
         <v>14</v>
       </c>
+      <c r="E543" t="s">
+        <v>9</v>
+      </c>
       <c r="F543" t="s">
         <v>10</v>
       </c>
@@ -10976,6 +11684,9 @@
       <c r="D544" t="s">
         <v>14</v>
       </c>
+      <c r="E544" t="s">
+        <v>9</v>
+      </c>
       <c r="F544" t="s">
         <v>10</v>
       </c>
@@ -10993,6 +11704,9 @@
       <c r="D545" t="s">
         <v>14</v>
       </c>
+      <c r="E545" t="s">
+        <v>9</v>
+      </c>
       <c r="F545" t="s">
         <v>10</v>
       </c>
@@ -11010,6 +11724,9 @@
       <c r="D546" t="s">
         <v>14</v>
       </c>
+      <c r="E546" t="s">
+        <v>9</v>
+      </c>
       <c r="F546" t="s">
         <v>21</v>
       </c>
@@ -11027,6 +11744,9 @@
       <c r="D547" t="s">
         <v>14</v>
       </c>
+      <c r="E547" t="s">
+        <v>9</v>
+      </c>
       <c r="F547" t="s">
         <v>10</v>
       </c>
@@ -11044,6 +11764,9 @@
       <c r="D548" t="s">
         <v>14</v>
       </c>
+      <c r="E548" t="s">
+        <v>9</v>
+      </c>
       <c r="F548" t="s">
         <v>10</v>
       </c>
@@ -11061,6 +11784,9 @@
       <c r="D549" t="s">
         <v>14</v>
       </c>
+      <c r="E549" t="s">
+        <v>9</v>
+      </c>
       <c r="F549" t="s">
         <v>10</v>
       </c>
@@ -11078,6 +11804,9 @@
       <c r="D550" t="s">
         <v>14</v>
       </c>
+      <c r="E550" t="s">
+        <v>9</v>
+      </c>
       <c r="F550" t="s">
         <v>10</v>
       </c>
@@ -11095,6 +11824,9 @@
       <c r="D551" t="s">
         <v>14</v>
       </c>
+      <c r="E551" t="s">
+        <v>9</v>
+      </c>
       <c r="F551" t="s">
         <v>21</v>
       </c>
@@ -11112,6 +11844,9 @@
       <c r="D552" t="s">
         <v>14</v>
       </c>
+      <c r="E552" t="s">
+        <v>9</v>
+      </c>
       <c r="F552" t="s">
         <v>10</v>
       </c>
@@ -11129,6 +11864,9 @@
       <c r="D553" t="s">
         <v>14</v>
       </c>
+      <c r="E553" t="s">
+        <v>9</v>
+      </c>
       <c r="F553" t="s">
         <v>10</v>
       </c>
@@ -11146,6 +11884,9 @@
       <c r="D554" t="s">
         <v>14</v>
       </c>
+      <c r="E554" t="s">
+        <v>9</v>
+      </c>
       <c r="F554" t="s">
         <v>10</v>
       </c>
@@ -11163,6 +11904,9 @@
       <c r="D555" t="s">
         <v>14</v>
       </c>
+      <c r="E555" t="s">
+        <v>9</v>
+      </c>
       <c r="F555" t="s">
         <v>10</v>
       </c>
@@ -11180,6 +11924,9 @@
       <c r="D556" t="s">
         <v>14</v>
       </c>
+      <c r="E556" t="s">
+        <v>9</v>
+      </c>
       <c r="F556" t="s">
         <v>10</v>
       </c>
@@ -11197,6 +11944,9 @@
       <c r="D557" t="s">
         <v>14</v>
       </c>
+      <c r="E557" t="s">
+        <v>9</v>
+      </c>
       <c r="F557" t="s">
         <v>10</v>
       </c>
@@ -11214,6 +11964,9 @@
       <c r="D558" t="s">
         <v>14</v>
       </c>
+      <c r="E558" t="s">
+        <v>9</v>
+      </c>
       <c r="F558" t="s">
         <v>10</v>
       </c>
@@ -11231,6 +11984,9 @@
       <c r="D559" t="s">
         <v>14</v>
       </c>
+      <c r="E559" t="s">
+        <v>9</v>
+      </c>
       <c r="F559" t="s">
         <v>10</v>
       </c>
@@ -11248,6 +12004,9 @@
       <c r="D560" t="s">
         <v>14</v>
       </c>
+      <c r="E560" t="s">
+        <v>9</v>
+      </c>
       <c r="F560" t="s">
         <v>21</v>
       </c>
@@ -11265,6 +12024,9 @@
       <c r="D561" t="s">
         <v>14</v>
       </c>
+      <c r="E561" t="s">
+        <v>9</v>
+      </c>
       <c r="F561" t="s">
         <v>10</v>
       </c>
@@ -11281,6 +12043,9 @@
       </c>
       <c r="D562" t="s">
         <v>14</v>
+      </c>
+      <c r="E562" t="s">
+        <v>9</v>
       </c>
       <c r="F562" t="s">
         <v>10</v>

</xml_diff>